<commit_message>
Completed initial version of the script.
</commit_message>
<xml_diff>
--- a/uft-one-sap-solution-manager-hosted-create-incident/Default.xlsx
+++ b/uft-one-sap-solution-manager-hosted-create-incident/Default.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+  <si>
+    <t>Don</t>
+  </si>
   <si>
     <t>EN - English</t>
   </si>
@@ -24,6 +27,9 @@
   </si>
   <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>IncidentPrefix</t>
   </si>
   <si>
     <t>bauera</t>
@@ -526,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -538,32 +544,39 @@
     <col min="2" max="2" width="9.80859375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.41796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.6171875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
       <c t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c t="s">
+        <v>3</v>
+      </c>
+      <c t="s">
+        <v>7</v>
       </c>
       <c t="s">
         <v>2</v>
       </c>
       <c t="s">
-        <v>5</v>
-      </c>
-      <c t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row>
       <c s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c s="1" t="s">
+        <v>1</v>
       </c>
       <c s="3" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Updated to run against all of the SAP Themes currently available, a competing solution uses images with pixel variances to identify objects, which breaks when you change themes.  This is to show that not only do we work with SAP UI5 (Fiori), with standard tiles, and standard SAP Solution Manager, but also that themes don't matter.
</commit_message>
<xml_diff>
--- a/uft-one-sap-solution-manager-hosted-create-incident/Default.xlsx
+++ b/uft-one-sap-solution-manager-hosted-create-incident/Default.xlsx
@@ -15,23 +15,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Don</t>
   </si>
   <si>
+    <t>SAP High Contrast Black (SAP Belize)</t>
+  </si>
+  <si>
     <t>EN - English</t>
   </si>
   <si>
     <t>Language</t>
   </si>
   <si>
+    <t>SAP Belize Deep</t>
+  </si>
+  <si>
+    <t>SAP Quartz Light</t>
+  </si>
+  <si>
+    <t>SAP Belize</t>
+  </si>
+  <si>
     <t>UserName</t>
   </si>
   <si>
     <t>IncidentPrefix</t>
   </si>
   <si>
+    <t>SAP High Contrast Black</t>
+  </si>
+  <si>
+    <t>SAP High Contrast White</t>
+  </si>
+  <si>
+    <t>SAP High Contrast White (SAP Belize)</t>
+  </si>
+  <si>
     <t>bauera</t>
   </si>
   <si>
@@ -45,6 +66,9 @@
   </si>
   <si>
     <t>https://www.sapsolutionmanagerdemo.com/sap/bc/ui5_ui5/ui2/ushell/shells/abap/FioriLaunchpad.html#Shell-home</t>
+  </si>
+  <si>
+    <t>Theme</t>
   </si>
 </sst>
 </file>
@@ -532,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -545,41 +569,168 @@
     <col min="3" max="3" width="9.41796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6171875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.078125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="30.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
       <c t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c t="s">
+        <v>7</v>
+      </c>
+      <c t="s">
+        <v>14</v>
       </c>
       <c t="s">
         <v>3</v>
       </c>
       <c t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c t="s">
-        <v>2</v>
-      </c>
-      <c t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row>
       <c s="1" t="s">
+        <v>16</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" t="s">
+        <v>0</v>
+      </c>
+      <c s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>16</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" t="s">
+        <v>0</v>
+      </c>
+      <c s="3" t="s">
         <v>9</v>
       </c>
-      <c s="1" t="s">
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>16</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" t="s">
+        <v>0</v>
+      </c>
+      <c s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>16</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" t="s">
+        <v>0</v>
+      </c>
+      <c s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>16</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" t="s">
+        <v>0</v>
+      </c>
+      <c s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>16</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" t="s">
+        <v>0</v>
+      </c>
+      <c s="3" t="s">
         <v>5</v>
       </c>
-      <c s="1" t="s">
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>16</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" t="s">
+        <v>0</v>
+      </c>
+      <c s="3" t="s">
         <v>6</v>
-      </c>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="3" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>